<commit_message>
Created two more test cases to test /getMe route. Successful tests.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95CF805-1DE9-4CC3-B8E9-538B5CCDD96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAD70D2-9057-44F6-8260-DF5189081439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="372">
   <si>
     <t>TC_ID</t>
   </si>
@@ -1194,6 +1194,50 @@
   </si>
   <si>
     <t>Manual API test via Postman. Confirms logout revokes access (client-side).</t>
+  </si>
+  <si>
+    <t>TC-057-API-17</t>
+  </si>
+  <si>
+    <t>TC-058-API-18</t>
+  </si>
+  <si>
+    <t>GET /api/auth/me returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>Server running GET /api/auth/me route exists; no token cookie present (logged out)</t>
+  </si>
+  <si>
+    <t>In Postman, ensure cookie jar does not include token for the API domain (or start a new session).
+Send GET /api/auth/me.</t>
+  </si>
+  <si>
+    <t>Returns 401 Unauthorized with JSON { success:false, message:'Not authorized.' } (or your exact middleware message)</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms requireAuth blocks unauthenticated requests and prevents controller execution.</t>
+  </si>
+  <si>
+    <t>Manual API test via Postman. Confirms session persists via HttpOnly cookie and req.user is populated from verified JWT.</t>
+  </si>
+  <si>
+    <t>GET /api/auth/me returns authenticated user context when logged in</t>
+  </si>
+  <si>
+    <t>Admin user exists; login works; token cookie present after login</t>
+  </si>
+  <si>
+    <t>Send POST /api/auth/login with valid admin credentials.
+Confirm login response is 200 and cookie token is set.
+Send GET /api/auth/me (same Postman session/cookie jar).</t>
+  </si>
+  <si>
+    <t>Login body: { "email": "&lt;ADMIN_USER&gt;", "password": "&lt;ADMIN_PASSWORD&gt;" }</t>
+  </si>
+  <si>
+    <t>GET /api/auth/me returns 200 OK with JSON:
+success: true
+data: { id: &lt;string&gt;, role: "Admin" }</t>
   </si>
 </sst>
 </file>
@@ -1620,11 +1664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N61" sqref="N61"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4003,6 +4047,97 @@
         <v>358</v>
       </c>
     </row>
+    <row r="58" spans="1:15" ht="75">
+      <c r="A58" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="K58" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N58" s="8">
+        <v>46040</v>
+      </c>
+      <c r="O58" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="120">
+      <c r="A59" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N59" s="8">
+        <v>46040</v>
+      </c>
+      <c r="O59" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Added test cases for admin routes to the spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033946DE-CA72-42BC-B84D-06754F543803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E2F087-1725-4C9F-A71E-9AC35BD8A504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1920" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="18000" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="479">
   <si>
     <t>TC_ID</t>
   </si>
@@ -1313,6 +1313,299 @@
   </si>
   <si>
     <t>Booking was created successfully (201) and saved with status = "Confirmed". App updated Booking smsStatus = "Sent" (provider accepted send request). Twilio Messaging Logs show the message ultimately Failed for the recipient number. Customer did not receive SMS.</t>
+  </si>
+  <si>
+    <t>TC-059-API-22</t>
+  </si>
+  <si>
+    <t>Admin GET /api/bookings/admin returns list of bookings (200) with populated service fields</t>
+  </si>
+  <si>
+    <t>Admin is authenticated (valid JWT cookie). At least 1 booking exists.</t>
+  </si>
+  <si>
+    <t>1) Login as admin to obtain auth cookie.
+2) Send GET /api/bookings/admin.
+3) Inspect response body.</t>
+  </si>
+  <si>
+    <t>Headers: Cookie=token=&lt;valid admin token&gt;
+Seed: Create booking(s) with serviceId, date, time.</t>
+  </si>
+  <si>
+    <t>200 OK. success=true. data is an array sorted by date/time. Each item includes serviceId populated with at least name and durationMins.</t>
+  </si>
+  <si>
+    <t>Verifies admin-only booking list endpoint.</t>
+  </si>
+  <si>
+    <t>TC-060-API-23</t>
+  </si>
+  <si>
+    <t>Admin GET /api/bookings/admin returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>No auth cookie present.</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/bookings/admin without auth cookie.
+2) Inspect response.</t>
+  </si>
+  <si>
+    <t>No Cookie header.</t>
+  </si>
+  <si>
+    <t>401 Unauthorized. success=false with auth error message.</t>
+  </si>
+  <si>
+    <t>requireAuth middleware.</t>
+  </si>
+  <si>
+    <t>TC-061-API-24</t>
+  </si>
+  <si>
+    <t>Admin GET /api/bookings/admin returns 403 when authenticated but not admin</t>
+  </si>
+  <si>
+    <t>User is authenticated but does not have admin role/flag.</t>
+  </si>
+  <si>
+    <t>1) Login as non-admin (or mock token with isAdmin=false).
+2) Send GET /api/bookings/admin.
+3) Inspect response.</t>
+  </si>
+  <si>
+    <t>Cookie=token=&lt;valid non-admin token&gt;</t>
+  </si>
+  <si>
+    <t>403 Forbidden. success=false with admin-only message.</t>
+  </si>
+  <si>
+    <t>adminOnly middleware.</t>
+  </si>
+  <si>
+    <t>TC-062-API-25</t>
+  </si>
+  <si>
+    <t>Admin POST /api/bookings/admin creates booking and sends SMS (smsStatus=Sent)</t>
+  </si>
+  <si>
+    <t>Admin authenticated. Target date/time is available per GET /availability. Twilio creds configured OR smsService mocked.</t>
+  </si>
+  <si>
+    <t>1) Login as admin.
+2) (Optional) GET /api/bookings/availability for date/serviceId; choose a returned time.
+3) POST /api/bookings/admin with valid payload.
+4) Inspect response and DB record.</t>
+  </si>
+  <si>
+    <t>POST body JSON:
+{
+  "serviceId": "&lt;valid&gt;",
+  "date": "YYYY-MM-DD",
+  "time": "10:00 AM",
+  "customerName": "Test Admin",
+  "phone": "+15555550100",
+  "email": "test@example.com",
+  "notes": "admin created"
+}</t>
+  </si>
+  <si>
+    <t>201 Created. success=true. data includes booking fields with status='Confirmed'. smsStatus becomes 'Sent' when SMS succeeds.</t>
+  </si>
+  <si>
+    <t>If running in dev without Twilio, mock smsService and assert DB fields.</t>
+  </si>
+  <si>
+    <t>TC-063-API-26</t>
+  </si>
+  <si>
+    <t>Admin POST /api/bookings/admin returns 409 for duplicate date/time</t>
+  </si>
+  <si>
+    <t>Admin authenticated. A booking already exists for the same date+time (unique index).</t>
+  </si>
+  <si>
+    <t>1) Ensure booking exists with date/time.
+2) Login as admin.
+3) POST /api/bookings/admin with same date/time.
+4) Inspect response.</t>
+  </si>
+  <si>
+    <t>POST body uses same date/time as existing booking.</t>
+  </si>
+  <si>
+    <t>409 Conflict. success=false. message='Slot already booked.'</t>
+  </si>
+  <si>
+    <t>Validates unique index handling and 11000 -&gt; 409 mapping.</t>
+  </si>
+  <si>
+    <t>TC-064-API-27</t>
+  </si>
+  <si>
+    <t>Admin POST /api/bookings/admin returns 404 when serviceId not found</t>
+  </si>
+  <si>
+    <t>Admin authenticated. Use a non-existent ObjectId for serviceId.</t>
+  </si>
+  <si>
+    <t>1) Login as admin.
+2) POST /api/bookings/admin with serviceId that does not exist.
+3) Inspect response.</t>
+  </si>
+  <si>
+    <t>serviceId="000000000000000000000000" (or any valid ObjectId not in DB).</t>
+  </si>
+  <si>
+    <t>404 Not Found. success=false. message='Service not found.'</t>
+  </si>
+  <si>
+    <t>Service integrity check.</t>
+  </si>
+  <si>
+    <t>TC-065-API-28</t>
+  </si>
+  <si>
+    <t>Admin PUT /api/bookings/admin/:id updates booking fields (200)</t>
+  </si>
+  <si>
+    <t>Admin authenticated. A booking exists. New date/time is available per GET /availability.</t>
+  </si>
+  <si>
+    <t>1) Create a booking (public or admin).
+2) Login as admin.
+3) PUT /api/bookings/admin/:id with updated payload.
+4) Inspect response and DB record.</t>
+  </si>
+  <si>
+    <t>PUT body JSON includes valid serviceId/date/time/customer fields. :id=&lt;existing booking id&gt;.</t>
+  </si>
+  <si>
+    <t>200 OK. success=true. data reflects updated fields and status remains 'Confirmed'.</t>
+  </si>
+  <si>
+    <t>Uses same schema as create; full payload required.</t>
+  </si>
+  <si>
+    <t>TC-066-API-29</t>
+  </si>
+  <si>
+    <t>Admin PUT /api/bookings/admin/:id returns 409 when updating to a duplicate date/time</t>
+  </si>
+  <si>
+    <t>Admin authenticated. Two bookings exist on same date; attempt to update one to the other's date/time.</t>
+  </si>
+  <si>
+    <t>1) Create Booking A at date/time.
+2) Create Booking B at different time.
+3) Login as admin.
+4) PUT Booking B to Booking A date/time.
+5) Inspect response.</t>
+  </si>
+  <si>
+    <t>PUT body sets date/time equal to an existing booking's date/time.</t>
+  </si>
+  <si>
+    <t>Validates unique index conflict on update.</t>
+  </si>
+  <si>
+    <t>TC-067-API-30</t>
+  </si>
+  <si>
+    <t>Admin PUT /api/bookings/admin/:id returns 404 when booking not found</t>
+  </si>
+  <si>
+    <t>Admin authenticated. Use a valid ObjectId not in bookings collection.</t>
+  </si>
+  <si>
+    <t>1) Login as admin.
+2) PUT /api/bookings/admin/:id with non-existent id.
+3) Inspect response.</t>
+  </si>
+  <si>
+    <t>:id="000000000000000000000000" (or any valid ObjectId not in DB).</t>
+  </si>
+  <si>
+    <t>404 Not Found. success=false. message='Booking not found.'</t>
+  </si>
+  <si>
+    <t>Find-by-id existence guard.</t>
+  </si>
+  <si>
+    <t>TC-068-API-31</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/bookings/admin/:id deletes booking (200) and booking is removed from list</t>
+  </si>
+  <si>
+    <t>Admin authenticated. A booking exists.</t>
+  </si>
+  <si>
+    <t>1) Create a booking.
+2) Login as admin.
+3) DELETE /api/bookings/admin/:id.
+4) GET /api/bookings/admin and verify it is no longer present.
+5) (Optional) GET /availability and verify time is available again.</t>
+  </si>
+  <si>
+    <t>:id=&lt;existing booking id&gt;</t>
+  </si>
+  <si>
+    <t>200 OK with success=true and message 'Booking deleted.' Booking no longer exists in DB and no longer appears in admin list.</t>
+  </si>
+  <si>
+    <t>Optional availability re-check verifies schedule freed.</t>
+  </si>
+  <si>
+    <t>TC-069-API-32</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/bookings/admin/:id returns 404 when booking not found</t>
+  </si>
+  <si>
+    <t>1) Login as admin.
+2) DELETE /api/bookings/admin/:id with non-existent id.
+3) Inspect response.</t>
+  </si>
+  <si>
+    <t>Delete existence guard.</t>
+  </si>
+  <si>
+    <t>TC-070-API-33</t>
+  </si>
+  <si>
+    <t>Admin POST /api/bookings/admin returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>1) POST /api/bookings/admin with valid payload but no auth cookie.
+2) Inspect response.</t>
+  </si>
+  <si>
+    <t>Valid booking JSON payload; no Cookie header.</t>
+  </si>
+  <si>
+    <t>requireAuth blocks admin create.</t>
+  </si>
+  <si>
+    <t>TC-071-API-34</t>
+  </si>
+  <si>
+    <t>Admin PUT /api/bookings/admin/:id returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>No auth cookie present. A booking exists.</t>
+  </si>
+  <si>
+    <t>1) Create a booking.
+2) PUT /api/bookings/admin/:id with valid payload but no auth cookie.
+3) Inspect response.</t>
+  </si>
+  <si>
+    <t>:id=&lt;existing booking id&gt;. Valid booking JSON payload; no Cookie header.</t>
+  </si>
+  <si>
+    <t>requireAuth blocks admin update.</t>
   </si>
 </sst>
 </file>
@@ -1428,11 +1721,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1446,7 +1746,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1754,11 +2068,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4369,22 +4683,648 @@
         <v>393</v>
       </c>
     </row>
+    <row r="63" spans="1:15" ht="90">
+      <c r="A63" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L63" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M63" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N63" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O63" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="45">
+      <c r="A64" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L64" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M64" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N64" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O64" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="60">
+      <c r="A65" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L65" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M65" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N65" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O65" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="225">
+      <c r="A66" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L66" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M66" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N66" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O66" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="75">
+      <c r="A67" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L67" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M67" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N67" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O67" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="60">
+      <c r="A68" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M68" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N68" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O68" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="75">
+      <c r="A69" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L69" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M69" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N69" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O69" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="75">
+      <c r="A70" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L70" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M70" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N70" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O70" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="60">
+      <c r="A71" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L71" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M71" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N71" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O71" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="105">
+      <c r="A72" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K72" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L72" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M72" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N72" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O72" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="60">
+      <c r="A73" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L73" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M73" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N73" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O73" s="5" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="45">
+      <c r="A74" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L74" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M74" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N74" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O74" s="5" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="60">
+      <c r="A75" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M75" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N75" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O75" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:O279">
-    <cfRule type="expression" dxfId="2" priority="4">
+  <conditionalFormatting sqref="A2:O62 A76:O123">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>$L2="Blocked"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:O62 A76:O279">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>$L2="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O123">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$L2="Blocked"</formula>
+  <conditionalFormatting sqref="A2:O62 A76:O316">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$L2="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O316">
+  <conditionalFormatting sqref="A63:O75">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$L63="Blocked"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:O75">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$L63="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:O75">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$L2="Failed"</formula>
+      <formula>$L63="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated the formal and markdown documents. Added test cases to the spreadsheet for messages and testimonials.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E2F087-1725-4C9F-A71E-9AC35BD8A504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF2BE03-7843-4DD4-8751-D0F10A070F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="18000" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="591">
   <si>
     <t>TC_ID</t>
   </si>
@@ -1606,6 +1606,345 @@
   </si>
   <si>
     <t>requireAuth blocks admin update.</t>
+  </si>
+  <si>
+    <t>TC-072-API-35</t>
+  </si>
+  <si>
+    <t>Public POST /api/messages creates a message (201)</t>
+  </si>
+  <si>
+    <t>API server running; MongoDB connected; message routes mounted at /api/messages.</t>
+  </si>
+  <si>
+    <t>1) Send POST /api/messages with valid body.</t>
+  </si>
+  <si>
+    <t>name='Jane Doe', phone='(916) 555-1234', email='jane@example.com', message='I would like to book a grooming appointment next week.'</t>
+  </si>
+  <si>
+    <t>201 Created; success=true; data contains _id, name, phone, email, message, createdAt.</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
+  <si>
+    <t>Planned manual API test (Postman)</t>
+  </si>
+  <si>
+    <t>TC-073-API-36</t>
+  </si>
+  <si>
+    <t>Public POST /api/messages returns 400 when required field missing</t>
+  </si>
+  <si>
+    <t>1) Send POST /api/messages with missing phone.</t>
+  </si>
+  <si>
+    <t>name='Jane Doe', email='jane@example.com', message='Hello there! (10+ chars)'</t>
+  </si>
+  <si>
+    <t>400 Bad Request; success=false; message explains missing required field (phone).</t>
+  </si>
+  <si>
+    <t>TC-074-API-37</t>
+  </si>
+  <si>
+    <t>Public POST /api/messages returns 400 for invalid phone characters</t>
+  </si>
+  <si>
+    <t>1) Send POST /api/messages with invalid phone (letters).</t>
+  </si>
+  <si>
+    <t>phone='abc-def-ghij', other fields valid</t>
+  </si>
+  <si>
+    <t>400 Bad Request; success=false; message indicates phone contains invalid characters / digit count invalid.</t>
+  </si>
+  <si>
+    <t>TC-075-API-38</t>
+  </si>
+  <si>
+    <t>Public POST /api/messages returns 400 for invalid email</t>
+  </si>
+  <si>
+    <t>1) Send POST /api/messages with invalid email format.</t>
+  </si>
+  <si>
+    <t>email='bad@', other fields valid</t>
+  </si>
+  <si>
+    <t>400 Bad Request; success=false; message indicates email must be valid.</t>
+  </si>
+  <si>
+    <t>TC-076-API-39</t>
+  </si>
+  <si>
+    <t>Admin GET /api/messages/admin returns list of messages (200)</t>
+  </si>
+  <si>
+    <t>Admin user exists; authenticated admin session/cookie; at least 2 messages exist in DB.</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/messages/admin with admin auth cookie.</t>
+  </si>
+  <si>
+    <t>200 OK; success=true; data is array of messages (can be empty) sorted newest-first (createdAt desc).</t>
+  </si>
+  <si>
+    <t>TC-077-API-40</t>
+  </si>
+  <si>
+    <t>Admin GET /api/messages/admin returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/messages/admin without auth cookie.</t>
+  </si>
+  <si>
+    <t>401 Unauthorized (or equivalent); success=false.</t>
+  </si>
+  <si>
+    <t>TC-078-API-41</t>
+  </si>
+  <si>
+    <t>Admin GET /api/messages/admin returns 403 when authenticated but not admin</t>
+  </si>
+  <si>
+    <t>Non-admin user authenticated (valid auth cookie) but lacks admin role.</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/messages/admin with non-admin auth cookie.</t>
+  </si>
+  <si>
+    <t>403 Forbidden; success=false.</t>
+  </si>
+  <si>
+    <t>TC-079-API-42</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/messages/admin/:id deletes message (200)</t>
+  </si>
+  <si>
+    <t>Admin authenticated; at least 1 message exists. Capture its _id.</t>
+  </si>
+  <si>
+    <t>1) Send DELETE /api/messages/admin/:id with admin auth cookie.
+2) Re-fetch GET /api/messages/admin.</t>
+  </si>
+  <si>
+    <t>id=&lt;existing message _id&gt;</t>
+  </si>
+  <si>
+    <t>200 OK; success=true; message indicates deletion. Deleted message no longer appears in list.</t>
+  </si>
+  <si>
+    <t>TC-080-API-43</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/messages/admin/:id returns 404 when message not found</t>
+  </si>
+  <si>
+    <t>Admin authenticated.</t>
+  </si>
+  <si>
+    <t>1) Send DELETE /api/messages/admin/:id with non-existent ObjectId.</t>
+  </si>
+  <si>
+    <t>id=&lt;valid but non-existent ObjectId&gt;</t>
+  </si>
+  <si>
+    <t>404 Not Found; success=false; message not found.</t>
+  </si>
+  <si>
+    <t>TC-081-API-44</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/messages/admin/:id returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>1) Send DELETE /api/messages/admin/:id without auth cookie.</t>
+  </si>
+  <si>
+    <t>id=&lt;any ObjectId&gt;</t>
+  </si>
+  <si>
+    <t>TC-082-API-45</t>
+  </si>
+  <si>
+    <t>Public GET /api/testimonials returns list (200)</t>
+  </si>
+  <si>
+    <t>API server running; MongoDB connected; testimonial routes mounted at /api/testimonials.</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/testimonials.</t>
+  </si>
+  <si>
+    <t>200 OK; success=true; data is array of testimonials (can be empty).</t>
+  </si>
+  <si>
+    <t>TC-083-API-46</t>
+  </si>
+  <si>
+    <t>Public GET /api/testimonials returns empty array when none exist</t>
+  </si>
+  <si>
+    <t>No testimonial documents exist in DB (or clear collection).</t>
+  </si>
+  <si>
+    <t>200 OK; success=true; data=[].</t>
+  </si>
+  <si>
+    <t>TC-084-API-47</t>
+  </si>
+  <si>
+    <t>Admin GET /api/testimonials/admin returns list (200)</t>
+  </si>
+  <si>
+    <t>Admin authenticated; testimonials exist in DB.</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/testimonials/admin with admin auth cookie.</t>
+  </si>
+  <si>
+    <t>TC-085-API-48</t>
+  </si>
+  <si>
+    <t>Admin GET /api/testimonials/admin returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/testimonials/admin without auth cookie.</t>
+  </si>
+  <si>
+    <t>TC-086-API-49</t>
+  </si>
+  <si>
+    <t>Admin GET /api/testimonials/admin returns 403 when authenticated but not admin</t>
+  </si>
+  <si>
+    <t>1) Send GET /api/testimonials/admin with non-admin auth cookie.</t>
+  </si>
+  <si>
+    <t>TC-087-API-50</t>
+  </si>
+  <si>
+    <t>Admin POST /api/testimonials/admin creates testimonial (201)</t>
+  </si>
+  <si>
+    <t>Admin authenticated; request body valid.</t>
+  </si>
+  <si>
+    <t>1) Send POST /api/testimonials/admin with valid body and admin auth cookie.</t>
+  </si>
+  <si>
+    <t>name='Sam', message='Fantastic groom and super friendly staff! Highly recommend.'</t>
+  </si>
+  <si>
+    <t>201 Created; success=true; data contains _id, name, message, createdAt.</t>
+  </si>
+  <si>
+    <t>TC-088-API-51</t>
+  </si>
+  <si>
+    <t>Admin POST /api/testimonials/admin returns 400 for invalid payload</t>
+  </si>
+  <si>
+    <t>1) Send POST /api/testimonials/admin with message shorter than 10 chars.</t>
+  </si>
+  <si>
+    <t>message='Too short'</t>
+  </si>
+  <si>
+    <t>400 Bad Request; success=false; message indicates minimum length.</t>
+  </si>
+  <si>
+    <t>TC-089-API-52</t>
+  </si>
+  <si>
+    <t>Admin PUT /api/testimonials/admin/:id updates testimonial (200)</t>
+  </si>
+  <si>
+    <t>Admin authenticated; testimonial exists. Capture its _id.</t>
+  </si>
+  <si>
+    <t>1) Send PUT /api/testimonials/admin/:id with one field (e.g., message).
+2) Re-fetch GET /api/testimonials/admin and confirm change.</t>
+  </si>
+  <si>
+    <t>id=&lt;existing testimonial _id&gt;, message='Updated testimonial message with 10+ chars'</t>
+  </si>
+  <si>
+    <t>200 OK; success=true; data reflects updated fields.</t>
+  </si>
+  <si>
+    <t>TC-090-API-53</t>
+  </si>
+  <si>
+    <t>Admin PUT /api/testimonials/admin/:id returns 400 when body is empty</t>
+  </si>
+  <si>
+    <t>Admin authenticated; testimonial exists.</t>
+  </si>
+  <si>
+    <t>1) Send PUT /api/testimonials/admin/:id with {}.</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>400 Bad Request; success=false; message indicates at least one field required.</t>
+  </si>
+  <si>
+    <t>TC-091-API-54</t>
+  </si>
+  <si>
+    <t>Admin PUT /api/testimonials/admin/:id returns 404 when testimonial not found</t>
+  </si>
+  <si>
+    <t>1) Send PUT /api/testimonials/admin/:id with non-existent ObjectId and valid body.</t>
+  </si>
+  <si>
+    <t>id=&lt;valid but non-existent ObjectId&gt;, message='Valid update message 10+ chars'</t>
+  </si>
+  <si>
+    <t>404 Not Found; success=false; message indicates testimonial not found.</t>
+  </si>
+  <si>
+    <t>TC-092-API-55</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/testimonials/admin/:id deletes testimonial (200) and returns deleted object</t>
+  </si>
+  <si>
+    <t>1) Send DELETE /api/testimonials/admin/:id with admin auth cookie.
+2) Re-fetch GET /api/testimonials/admin.</t>
+  </si>
+  <si>
+    <t>id=&lt;existing testimonial _id&gt;</t>
+  </si>
+  <si>
+    <t>200 OK; success=true; data is deleted testimonial; it no longer appears in list.</t>
+  </si>
+  <si>
+    <t>TC-093-API-56</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/testimonials/admin/:id returns 404 when testimonial not found</t>
+  </si>
+  <si>
+    <t>1) Send DELETE /api/testimonials/admin/:id with non-existent ObjectId.</t>
+  </si>
+  <si>
+    <t>404 Not Found; success=false; message indicates not found.</t>
+  </si>
+  <si>
+    <t>TC-094-API-57</t>
+  </si>
+  <si>
+    <t>Admin DELETE /api/testimonials/admin/:id returns 401 when not authenticated</t>
+  </si>
+  <si>
+    <t>1) Send DELETE /api/testimonials/admin/:id without auth cookie.</t>
   </si>
 </sst>
 </file>
@@ -2068,11 +2407,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O75"/>
+  <dimension ref="A1:O98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5294,37 +5633,1026 @@
         <v>478</v>
       </c>
     </row>
+    <row r="76" spans="1:15" ht="90">
+      <c r="A76" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L76" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="60">
+      <c r="A77" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L77" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="60">
+      <c r="A78" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L78" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="45">
+      <c r="A79" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="K79" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L79" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="60">
+      <c r="A80" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L80" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="30">
+      <c r="A81" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="K81" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L81" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="30">
+      <c r="A82" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="K82" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L82" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="45">
+      <c r="A83" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L83" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="30">
+      <c r="A84" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="K84" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L84" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="30">
+      <c r="A85" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="K85" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L85" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="30">
+      <c r="A86" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="I86" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="K86" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L86" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+      <c r="O86" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="30">
+      <c r="A87" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L87" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+      <c r="O87" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="30">
+      <c r="A88" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M88" s="5"/>
+      <c r="N88" s="5"/>
+      <c r="O88" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="30">
+      <c r="A89" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L89" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M89" s="5"/>
+      <c r="N89" s="5"/>
+      <c r="O89" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="45">
+      <c r="A90" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="K90" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L90" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="75">
+      <c r="A91" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="K91" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L91" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+      <c r="O91" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="45">
+      <c r="A92" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="K92" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L92" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="60">
+      <c r="A93" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L93" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+      <c r="O93" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" ht="45">
+      <c r="A94" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L94" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" ht="60">
+      <c r="A95" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L95" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+      <c r="O95" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="45">
+      <c r="A96" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="K96" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L96" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="30">
+      <c r="A97" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="K97" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L97" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="30">
+      <c r="A98" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="K98" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="L98" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M98" s="5"/>
+      <c r="N98" s="5"/>
+      <c r="O98" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:O62 A76:O123">
-    <cfRule type="expression" dxfId="5" priority="6">
+  <conditionalFormatting sqref="A2:O75 A99:O123">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$L2="Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O62 A76:O279">
-    <cfRule type="expression" dxfId="4" priority="7">
+  <conditionalFormatting sqref="A2:O75 A99:O279">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$L2="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O62 A76:O316">
+  <conditionalFormatting sqref="A2:O75 A99:O316">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$L2="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:O75">
+  <conditionalFormatting sqref="A76:O98">
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$L63="Blocked"</formula>
+      <formula>$L76="Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:O75">
+  <conditionalFormatting sqref="A76:O98">
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$L63="Pass"</formula>
+      <formula>$L76="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:O75">
+  <conditionalFormatting sqref="A76:O98">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$L63="Failed"</formula>
+      <formula>$L76="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ran test cases and updated spreadsheet. Refactored the delete controller funcs for messages and bookings.
</commit_message>
<xml_diff>
--- a/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
+++ b/docs/formal/Test_Cases_V1_with_Service_API_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF2BE03-7843-4DD4-8751-D0F10A070F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15F4F7F-142D-4DF6-9365-CFA171DE0556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="584">
   <si>
     <t>TC_ID</t>
   </si>
@@ -1359,29 +1359,6 @@
   </si>
   <si>
     <t>requireAuth middleware.</t>
-  </si>
-  <si>
-    <t>TC-061-API-24</t>
-  </si>
-  <si>
-    <t>Admin GET /api/bookings/admin returns 403 when authenticated but not admin</t>
-  </si>
-  <si>
-    <t>User is authenticated but does not have admin role/flag.</t>
-  </si>
-  <si>
-    <t>1) Login as non-admin (or mock token with isAdmin=false).
-2) Send GET /api/bookings/admin.
-3) Inspect response.</t>
-  </si>
-  <si>
-    <t>Cookie=token=&lt;valid non-admin token&gt;</t>
-  </si>
-  <si>
-    <t>403 Forbidden. success=false with admin-only message.</t>
-  </si>
-  <si>
-    <t>adminOnly middleware.</t>
   </si>
   <si>
     <t>TC-062-API-25</t>
@@ -2060,28 +2037,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -2407,11 +2363,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5041,31 +4997,31 @@
       <c r="F63" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="5" t="s">
+      <c r="G63" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H63" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="I63" s="5" t="s">
+      <c r="I63" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="J63" s="5" t="s">
+      <c r="J63" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="K63" s="5" t="s">
-        <v>23</v>
+      <c r="K63" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L63" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M63" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N63" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O63" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N63" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O63" s="7" t="s">
         <v>401</v>
       </c>
     </row>
@@ -5088,40 +5044,40 @@
       <c r="F64" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G64" s="5" t="s">
+      <c r="G64" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I64" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="J64" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="K64" s="5" t="s">
-        <v>23</v>
+      <c r="K64" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M64" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N64" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O64" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N64" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O64" s="7" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="60">
+    <row r="65" spans="1:15" ht="225">
       <c r="A65" s="7" t="s">
         <v>409</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>410</v>
@@ -5130,40 +5086,40 @@
         <v>255</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G65" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G65" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I65" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="J65" s="5" t="s">
+      <c r="J65" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="K65" s="5" t="s">
-        <v>23</v>
+      <c r="K65" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M65" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N65" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O65" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N65" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O65" s="7" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="225">
+    <row r="66" spans="1:15" ht="75">
       <c r="A66" s="7" t="s">
         <v>416</v>
       </c>
@@ -5177,40 +5133,40 @@
         <v>255</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G66" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G66" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I66" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="J66" s="5" t="s">
+      <c r="J66" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="K66" s="5" t="s">
-        <v>23</v>
+      <c r="K66" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M66" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N66" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O66" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N66" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O66" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="75">
+    <row r="67" spans="1:15" ht="60">
       <c r="A67" s="7" t="s">
         <v>423</v>
       </c>
@@ -5224,40 +5180,40 @@
         <v>255</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G67" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H67" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I67" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="J67" s="5" t="s">
+      <c r="J67" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="K67" s="5" t="s">
-        <v>23</v>
+      <c r="K67" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L67" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M67" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N67" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O67" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N67" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O67" s="7" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="60">
+    <row r="68" spans="1:15" ht="75">
       <c r="A68" s="7" t="s">
         <v>430</v>
       </c>
@@ -5271,36 +5227,36 @@
         <v>255</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G68" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G68" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I68" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="J68" s="5" t="s">
+      <c r="J68" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K68" s="5" t="s">
-        <v>23</v>
+      <c r="K68" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L68" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M68" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N68" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O68" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N68" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O68" s="7" t="s">
         <v>436</v>
       </c>
     </row>
@@ -5318,87 +5274,87 @@
         <v>255</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G69" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I69" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="J69" s="5" t="s">
+      <c r="J69" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="K69" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L69" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M69" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N69" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O69" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="K69" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L69" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M69" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N69" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O69" s="5" t="s">
+    </row>
+    <row r="70" spans="1:15" ht="60">
+      <c r="A70" s="7" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="75">
-      <c r="A70" s="7" t="s">
-        <v>444</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>198</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>255</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G70" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="H70" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="I70" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="J70" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="J70" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="K70" s="5" t="s">
-        <v>23</v>
+      <c r="K70" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M70" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N70" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O70" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N70" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O70" s="7" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="60">
+    <row r="71" spans="1:15" ht="105">
       <c r="A71" s="7" t="s">
         <v>450</v>
       </c>
@@ -5412,40 +5368,40 @@
         <v>255</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G71" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G71" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H71" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="J71" s="5" t="s">
+      <c r="J71" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="K71" s="5" t="s">
-        <v>23</v>
+      <c r="K71" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>25</v>
+        <v>260</v>
       </c>
       <c r="M71" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N71" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O71" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N71" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O71" s="7" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="105">
+    <row r="72" spans="1:15" ht="60">
       <c r="A72" s="7" t="s">
         <v>457</v>
       </c>
@@ -5459,1200 +5415,1140 @@
         <v>255</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G72" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="H72" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="I72" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="K72" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L72" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M72" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N72" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O72" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="I72" s="5" t="s">
+    </row>
+    <row r="73" spans="1:15" ht="45">
+      <c r="A73" s="7" t="s">
         <v>461</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="K72" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L72" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M72" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N72" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O72" s="5" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="60">
-      <c r="A73" s="7" t="s">
-        <v>464</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>198</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>255</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G73" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="H73" s="5" t="s">
+      <c r="G73" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="K73" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L73" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M73" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N73" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O73" s="7" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="60">
+      <c r="A74" s="7" t="s">
         <v>466</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="J73" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="K73" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L73" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M73" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N73" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O73" s="5" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="45">
-      <c r="A74" s="7" t="s">
-        <v>468</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>198</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>255</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G74" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="H74" s="5" t="s">
+      <c r="G74" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="I74" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="I74" s="5" t="s">
+      <c r="J74" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="K74" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L74" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M74" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N74" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O74" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="J74" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="K74" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L74" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M74" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N74" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O74" s="5" t="s">
+    </row>
+    <row r="75" spans="1:15" ht="90">
+      <c r="A75" s="7" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" ht="60">
-      <c r="A75" s="7" t="s">
+      <c r="B75" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" s="7" t="s">
         <v>473</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>474</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>255</v>
       </c>
       <c r="E75" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M75" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N75" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O75" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="60">
+      <c r="A76" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E76" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F75" s="7" t="s">
+      <c r="F76" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G75" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="K75" s="5" t="s">
+      <c r="G76" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="J76" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="K76" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L76" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M76" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N76" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O76" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="60">
+      <c r="A77" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="K77" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L77" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M77" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N77" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O77" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="45">
+      <c r="A78" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="K78" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L78" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M78" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N78" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O78" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="60">
+      <c r="A79" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="I79" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L75" s="7" t="s">
+      <c r="J79" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="K79" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L79" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M79" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N79" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O79" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="30">
+      <c r="A80" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G80" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="I80" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J80" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="K80" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L80" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M80" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N80" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O80" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="30" hidden="1">
+      <c r="A81" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="I81" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J81" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="K81" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L81" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M75" s="7" t="s">
+      <c r="O81" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="45">
+      <c r="A82" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="K82" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L82" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M82" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N82" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O82" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="30">
+      <c r="A83" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="I83" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="J83" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="K83" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L83" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M83" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N83" s="8">
+        <v>46063</v>
+      </c>
+      <c r="O83" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="30">
+      <c r="A84" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="J84" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="K84" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L84" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O84" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="30">
+      <c r="A85" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="I85" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N75" s="8" t="s">
+      <c r="J85" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="K85" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L85" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O85" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="30">
+      <c r="A86" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="I86" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O75" s="5" t="s">
+      <c r="J86" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="K86" s="7" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" ht="90">
-      <c r="A76" s="5" t="s">
+      <c r="L86" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O86" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="D76" s="5" t="s">
+    </row>
+    <row r="87" spans="1:15" ht="30">
+      <c r="A87" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="D87" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L76" s="5" t="s">
+      <c r="E87" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J87" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="K87" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L87" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
-      <c r="O76" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="60">
-      <c r="A77" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="D77" s="5" t="s">
+      <c r="O87" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="30">
+      <c r="A88" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E88" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J88" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="K88" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L88" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O88" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="45">
+      <c r="A89" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J89" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="K89" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L89" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O89" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="75">
+      <c r="A90" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="H90" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="J90" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="K90" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L90" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O90" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="45">
+      <c r="A91" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E91" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F91" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G77" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="K77" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L77" s="5" t="s">
+      <c r="G91" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="K91" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L91" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M77" s="5"/>
-      <c r="N77" s="5"/>
-      <c r="O77" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="60">
-      <c r="A78" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="D78" s="5" t="s">
+      <c r="O91" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="60">
+      <c r="A92" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E92" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="H92" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="I92" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="J92" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="K92" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L92" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O92" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="45">
+      <c r="A93" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E93" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F93" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G78" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="I78" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="J78" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="K78" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L78" s="5" t="s">
+      <c r="G93" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="I93" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="K93" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L93" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M78" s="5"/>
-      <c r="N78" s="5"/>
-      <c r="O78" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="45">
-      <c r="A79" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="D79" s="5" t="s">
+      <c r="O93" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" ht="60">
+      <c r="A94" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="D94" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E94" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F94" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G79" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="J79" s="5" t="s">
-        <v>501</v>
-      </c>
-      <c r="K79" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L79" s="5" t="s">
+      <c r="G94" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="H94" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="J94" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="K94" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L94" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="60">
-      <c r="A80" s="5" t="s">
-        <v>502</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C80" s="5" t="s">
+      <c r="O94" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" ht="45">
+      <c r="A95" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="J95" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="K95" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L95" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O95" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="30">
+      <c r="A96" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="H96" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="I96" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="J96" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="K96" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L96" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O96" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="30">
+      <c r="A97" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="I97" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="J97" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="K80" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L80" s="5" t="s">
+      <c r="K97" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="L97" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="30">
-      <c r="A81" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J81" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="K81" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L81" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="30">
-      <c r="A82" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>514</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J82" s="5" t="s">
-        <v>515</v>
-      </c>
-      <c r="K82" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L82" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="45">
-      <c r="A83" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>519</v>
-      </c>
-      <c r="I83" s="5" t="s">
-        <v>520</v>
-      </c>
-      <c r="J83" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="K83" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L83" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5"/>
-      <c r="O83" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="30">
-      <c r="A84" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="H84" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>526</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="K84" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L84" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M84" s="5"/>
-      <c r="N84" s="5"/>
-      <c r="O84" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" ht="30">
-      <c r="A85" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>529</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H85" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="K85" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L85" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M85" s="5"/>
-      <c r="N85" s="5"/>
-      <c r="O85" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="30">
-      <c r="A86" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>533</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>535</v>
-      </c>
-      <c r="I86" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J86" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="K86" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L86" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M86" s="5"/>
-      <c r="N86" s="5"/>
-      <c r="O86" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="30">
-      <c r="A87" s="5" t="s">
-        <v>537</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>538</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>539</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>535</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="K87" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L87" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M87" s="5"/>
-      <c r="N87" s="5"/>
-      <c r="O87" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="30">
-      <c r="A88" s="5" t="s">
-        <v>541</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>542</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>543</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>544</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L88" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" ht="30">
-      <c r="A89" s="5" t="s">
-        <v>545</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>546</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>547</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="K89" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L89" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M89" s="5"/>
-      <c r="N89" s="5"/>
-      <c r="O89" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" ht="45">
-      <c r="A90" s="5" t="s">
-        <v>548</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>549</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>550</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>515</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L90" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M90" s="5"/>
-      <c r="N90" s="5"/>
-      <c r="O90" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" ht="75">
-      <c r="A91" s="5" t="s">
-        <v>551</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>553</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>554</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L91" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M91" s="5"/>
-      <c r="N91" s="5"/>
-      <c r="O91" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" ht="45">
-      <c r="A92" s="5" t="s">
-        <v>557</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>558</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G92" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>559</v>
-      </c>
-      <c r="I92" s="5" t="s">
-        <v>560</v>
-      </c>
-      <c r="J92" s="5" t="s">
-        <v>561</v>
-      </c>
-      <c r="K92" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L92" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M92" s="5"/>
-      <c r="N92" s="5"/>
-      <c r="O92" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" ht="60">
-      <c r="A93" s="5" t="s">
-        <v>562</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G93" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="I93" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="J93" s="5" t="s">
-        <v>567</v>
-      </c>
-      <c r="K93" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L93" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M93" s="5"/>
-      <c r="N93" s="5"/>
-      <c r="O93" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" ht="45">
-      <c r="A94" s="5" t="s">
-        <v>568</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>569</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G94" s="5" t="s">
-        <v>570</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>571</v>
-      </c>
-      <c r="I94" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="J94" s="5" t="s">
-        <v>573</v>
-      </c>
-      <c r="K94" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L94" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" ht="60">
-      <c r="A95" s="5" t="s">
-        <v>574</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>576</v>
-      </c>
-      <c r="I95" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="J95" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="K95" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L95" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M95" s="5"/>
-      <c r="N95" s="5"/>
-      <c r="O95" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" ht="45">
-      <c r="A96" s="5" t="s">
-        <v>579</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>580</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="I96" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="J96" s="5" t="s">
-        <v>583</v>
-      </c>
-      <c r="K96" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L96" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M96" s="5"/>
-      <c r="N96" s="5"/>
-      <c r="O96" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="30">
-      <c r="A97" s="5" t="s">
-        <v>584</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>585</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="I97" s="5" t="s">
-        <v>526</v>
-      </c>
-      <c r="J97" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="K97" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L97" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M97" s="5"/>
-      <c r="N97" s="5"/>
-      <c r="O97" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" ht="30">
-      <c r="A98" s="5" t="s">
-        <v>588</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="I98" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="J98" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="K98" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L98" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M98" s="5"/>
-      <c r="N98" s="5"/>
-      <c r="O98" s="5" t="s">
-        <v>486</v>
+      <c r="O97" s="7" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:O49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:O75 A99:O123">
-    <cfRule type="expression" dxfId="5" priority="5">
+  <conditionalFormatting sqref="A2:O122">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$L2="Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O75 A99:O279">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="A2:O278">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$L2="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O75 A99:O316">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="A2:O315">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$L2="Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76:O98">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$L76="Blocked"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76:O98">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$L76="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A76:O98">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$L76="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>